<commit_message>
brand names were wrong; fixed
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haedongkim/OneDrive - The Pennsylvania State University/PSU/2018_fall/IE511_DOE/doe_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="102_{2797EF77-0756-A34C-8D24-034C0825A29B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{CDCCED59-373B-4541-BFE1-0FAC2F629AAD}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="102_{2797EF77-0756-A34C-8D24-034C0825A29B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B1EFA1F5-44D0-C648-8F88-5F5E710283FE}"/>
   <bookViews>
     <workbookView xWindow="8460" yWindow="460" windowWidth="16680" windowHeight="12180" xr2:uid="{46B79356-C417-3945-AC40-44D925216AD9}"/>
   </bookViews>
@@ -599,7 +599,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -684,10 +684,10 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
         <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -1174,7 +1174,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>